<commit_message>
add data nico and partial figures for the meeting
</commit_message>
<xml_diff>
--- a/results/tables/pairs.xlsx
+++ b/results/tables/pairs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/diego_kozlowski/GIT/1_scinet/mobility/topics_mobility/mobility-topic/results/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6420A3E7-3E4F-E345-874A-3727E93AF627}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B9EF5A7-98A2-6745-A9C2-5504B737C14D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5460" yWindow="-21100" windowWidth="19200" windowHeight="21100" xr2:uid="{F09397FE-FF22-FF42-A3EA-56D5573B3C83}"/>
+    <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17440" xr2:uid="{F09397FE-FF22-FF42-A3EA-56D5573B3C83}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="40">
   <si>
     <t>country</t>
   </si>
@@ -44,36 +44,18 @@
     <t>cosine</t>
   </si>
   <si>
-    <t>Emigrant Immigrant</t>
-  </si>
-  <si>
-    <t>United Kingdom</t>
-  </si>
-  <si>
     <t>Germany</t>
   </si>
   <si>
-    <t>Switzerland</t>
-  </si>
-  <si>
-    <t>Brazil</t>
-  </si>
-  <si>
     <t>China</t>
   </si>
   <si>
-    <t>United States</t>
-  </si>
-  <si>
     <t>Netherlands</t>
   </si>
   <si>
     <t>Japan</t>
   </si>
   <si>
-    <t>India</t>
-  </si>
-  <si>
     <t>Canada</t>
   </si>
   <si>
@@ -116,9 +98,6 @@
     <t>Thailand</t>
   </si>
   <si>
-    <t>New Zealand</t>
-  </si>
-  <si>
     <t>Jordan</t>
   </si>
   <si>
@@ -161,9 +140,6 @@
     <t>United Arab Emirates</t>
   </si>
   <si>
-    <t>Latvia</t>
-  </si>
-  <si>
     <t>Countries with most similar pairs</t>
   </si>
   <si>
@@ -171,6 +147,15 @@
   </si>
   <si>
     <t>total publications</t>
+  </si>
+  <si>
+    <t>Iraq</t>
+  </si>
+  <si>
+    <t>North Macedonia</t>
+  </si>
+  <si>
+    <t>Zimbabwe</t>
   </si>
 </sst>
 </file>
@@ -348,6 +333,24 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -358,24 +361,6 @@
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -698,10 +683,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{344B62AC-2443-6C45-A1DF-299F97BFEB0B}">
-  <dimension ref="A1:G35"/>
+  <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G35" sqref="A1:G35"/>
+      <selection sqref="A1:G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -717,201 +702,201 @@
   <sheetData>
     <row r="1" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="B1" s="14"/>
       <c r="C1" s="14"/>
       <c r="D1" s="15"/>
       <c r="E1" s="14" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="F1" s="14"/>
       <c r="G1" s="14"/>
     </row>
-    <row r="2" spans="1:7" ht="32" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:7" ht="32" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>44</v>
+      <c r="C2" s="11" t="s">
+        <v>36</v>
       </c>
       <c r="D2" s="13"/>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="5" t="s">
-        <v>44</v>
+      <c r="G2" s="11" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="19" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="4"/>
+      <c r="G3" s="5"/>
+    </row>
+    <row r="4" spans="1:7" ht="18" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="11"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="F3" s="11"/>
-      <c r="G3" s="12"/>
-    </row>
-    <row r="4" spans="1:7" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>3</v>
-      </c>
       <c r="B4" s="2">
-        <v>0.96</v>
+        <v>0.94</v>
       </c>
       <c r="C4" s="2">
-        <v>2322672</v>
-      </c>
-      <c r="D4" s="6"/>
+        <v>1979964</v>
+      </c>
+      <c r="D4" s="12"/>
       <c r="E4" s="1" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="F4" s="2">
-        <v>0.12</v>
+        <v>0.08</v>
       </c>
       <c r="G4" s="2">
-        <v>13885</v>
+        <v>18628</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B5" s="2">
-        <v>0.95</v>
+        <v>0.93</v>
       </c>
       <c r="C5" s="2">
-        <v>1979964</v>
-      </c>
-      <c r="D5" s="6"/>
+        <v>33552</v>
+      </c>
+      <c r="D5" s="12"/>
       <c r="E5" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F5" s="2">
-        <v>0.13</v>
+        <v>0.17</v>
       </c>
       <c r="G5" s="2">
-        <v>27385</v>
+        <v>31256</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B6" s="2">
-        <v>0.94</v>
+        <v>0.93</v>
       </c>
       <c r="C6" s="2">
-        <v>543900</v>
-      </c>
-      <c r="D6" s="6"/>
+        <v>131337</v>
+      </c>
+      <c r="D6" s="12"/>
       <c r="E6" s="1" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="F6" s="2">
-        <v>0.18</v>
+        <v>0.22</v>
       </c>
       <c r="G6" s="2">
-        <v>31256</v>
+        <v>13361</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B7" s="2">
-        <v>0.94</v>
+        <v>0.93</v>
       </c>
       <c r="C7" s="2">
-        <v>828726</v>
-      </c>
-      <c r="D7" s="6"/>
+        <v>86826</v>
+      </c>
+      <c r="D7" s="12"/>
       <c r="E7" s="1" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="F7" s="2">
-        <v>0.2</v>
+        <v>0.23</v>
       </c>
       <c r="G7" s="2">
-        <v>18628</v>
+        <v>57420</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B8" s="2">
-        <v>0.93</v>
+        <v>0.92</v>
       </c>
       <c r="C8" s="2">
-        <v>4610029</v>
-      </c>
-      <c r="D8" s="6"/>
+        <v>175730</v>
+      </c>
+      <c r="D8" s="12"/>
       <c r="E8" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="F8" s="2">
-        <v>0.21</v>
+        <v>0.24</v>
       </c>
       <c r="G8" s="2">
-        <v>41158</v>
+        <v>16738</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B9" s="2">
-        <v>0.92</v>
+        <v>0.91</v>
       </c>
       <c r="C9" s="2">
-        <v>7631237</v>
-      </c>
-      <c r="D9" s="6"/>
+        <v>703548</v>
+      </c>
+      <c r="D9" s="12"/>
       <c r="E9" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F9" s="2">
-        <v>0.22</v>
+        <v>0.24</v>
       </c>
       <c r="G9" s="2">
-        <v>10548</v>
+        <v>6682</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="B10" s="2">
-        <v>0.91</v>
+        <v>0.9</v>
       </c>
       <c r="C10" s="2">
-        <v>703548</v>
-      </c>
-      <c r="D10" s="6"/>
+        <v>4610029</v>
+      </c>
+      <c r="D10" s="12"/>
       <c r="E10" s="1" t="s">
         <v>23</v>
       </c>
       <c r="F10" s="2">
-        <v>0.25</v>
+        <v>0.24</v>
       </c>
       <c r="G10" s="2">
-        <v>57420</v>
+        <v>43257</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B11" s="2">
         <v>0.9</v>
@@ -919,33 +904,33 @@
       <c r="C11" s="2">
         <v>1565285</v>
       </c>
-      <c r="D11" s="6"/>
+      <c r="D11" s="12"/>
       <c r="E11" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F11" s="2">
-        <v>0.28999999999999998</v>
+        <v>0.26</v>
       </c>
       <c r="G11" s="2">
-        <v>13038</v>
+        <v>5182</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B12" s="2">
-        <v>0.9</v>
+        <v>0.89</v>
       </c>
       <c r="C12" s="2">
-        <v>1214410</v>
-      </c>
-      <c r="D12" s="6"/>
+        <v>90813</v>
+      </c>
+      <c r="D12" s="12"/>
       <c r="E12" s="1" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="F12" s="2">
-        <v>0.3</v>
+        <v>0.27</v>
       </c>
       <c r="G12" s="2">
         <v>23244</v>
@@ -953,188 +938,188 @@
     </row>
     <row r="13" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B13" s="2">
-        <v>0.89</v>
+        <v>0.88</v>
       </c>
       <c r="C13" s="2">
-        <v>1288629</v>
-      </c>
-      <c r="D13" s="6"/>
+        <v>426195</v>
+      </c>
+      <c r="D13" s="12"/>
       <c r="E13" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="F13" s="2">
-        <v>0.31</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="G13" s="2">
-        <v>30629</v>
+        <v>10548</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" s="8"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F14" s="8"/>
-      <c r="G14" s="9"/>
-    </row>
-    <row r="15" spans="1:7" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="7"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F14" s="7"/>
+      <c r="G14" s="8"/>
+    </row>
+    <row r="15" spans="1:7" ht="18" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="B15" s="2">
-        <v>0.94</v>
+        <v>0.93</v>
       </c>
       <c r="C15" s="2">
-        <v>1979964</v>
-      </c>
-      <c r="D15" s="6"/>
+        <v>193916</v>
+      </c>
+      <c r="D15" s="12"/>
       <c r="E15" s="1" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="F15" s="2">
-        <v>0.08</v>
+        <v>0.05</v>
       </c>
       <c r="G15" s="2">
-        <v>18628</v>
+        <v>8743</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="B16" s="2">
-        <v>0.93</v>
+        <v>0.92</v>
       </c>
       <c r="C16" s="2">
-        <v>33552</v>
-      </c>
-      <c r="D16" s="6"/>
+        <v>4610029</v>
+      </c>
+      <c r="D16" s="12"/>
       <c r="E16" s="1" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="F16" s="2">
-        <v>0.17</v>
+        <v>0.1</v>
       </c>
       <c r="G16" s="2">
-        <v>31256</v>
+        <v>27385</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B17" s="2">
-        <v>0.93</v>
+        <v>0.92</v>
       </c>
       <c r="C17" s="2">
-        <v>131337</v>
-      </c>
-      <c r="D17" s="6"/>
+        <v>84039</v>
+      </c>
+      <c r="D17" s="12"/>
       <c r="E17" s="1" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="F17" s="2">
-        <v>0.22</v>
+        <v>0.18</v>
       </c>
       <c r="G17" s="2">
-        <v>13361</v>
+        <v>41158</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B18" s="2">
-        <v>0.93</v>
+        <v>0.91</v>
       </c>
       <c r="C18" s="2">
-        <v>86826</v>
-      </c>
-      <c r="D18" s="6"/>
+        <v>57420</v>
+      </c>
+      <c r="D18" s="12"/>
       <c r="E18" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="F18" s="2">
-        <v>0.24</v>
+        <v>0.21</v>
       </c>
       <c r="G18" s="2">
-        <v>57420</v>
+        <v>13885</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="B19" s="2">
-        <v>0.92</v>
+        <v>0.9</v>
       </c>
       <c r="C19" s="2">
-        <v>175730</v>
-      </c>
-      <c r="D19" s="6"/>
+        <v>1979964</v>
+      </c>
+      <c r="D19" s="12"/>
       <c r="E19" s="1" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="F19" s="2">
-        <v>0.24</v>
+        <v>0.22</v>
       </c>
       <c r="G19" s="2">
-        <v>16738</v>
+        <v>30629</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B20" s="2">
-        <v>0.91</v>
+        <v>0.9</v>
       </c>
       <c r="C20" s="2">
-        <v>703548</v>
-      </c>
-      <c r="D20" s="6"/>
+        <v>1288629</v>
+      </c>
+      <c r="D20" s="12"/>
       <c r="E20" s="1" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="F20" s="2">
-        <v>0.24</v>
+        <v>0.23</v>
       </c>
       <c r="G20" s="2">
-        <v>43257</v>
+        <v>18628</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B21" s="2">
         <v>0.9</v>
       </c>
       <c r="C21" s="2">
-        <v>4610029</v>
-      </c>
-      <c r="D21" s="6"/>
+        <v>703548</v>
+      </c>
+      <c r="D21" s="12"/>
       <c r="E21" s="1" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="F21" s="2">
-        <v>0.27</v>
+        <v>0.26</v>
       </c>
       <c r="G21" s="2">
-        <v>23244</v>
+        <v>43257</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B22" s="2">
         <v>0.9</v>
@@ -1142,15 +1127,15 @@
       <c r="C22" s="2">
         <v>1565285</v>
       </c>
-      <c r="D22" s="6"/>
+      <c r="D22" s="12"/>
       <c r="E22" s="1" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="F22" s="2">
-        <v>0.28000000000000003</v>
+        <v>0.31</v>
       </c>
       <c r="G22" s="2">
-        <v>10548</v>
+        <v>51462</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="31" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -1161,17 +1146,17 @@
         <v>0.89</v>
       </c>
       <c r="C23" s="2">
-        <v>90813</v>
-      </c>
-      <c r="D23" s="6"/>
+        <v>19328</v>
+      </c>
+      <c r="D23" s="12"/>
       <c r="E23" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="F23" s="2">
-        <v>0.33</v>
+        <v>0.37</v>
       </c>
       <c r="G23" s="2">
-        <v>29084</v>
+        <v>71464</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -1179,255 +1164,31 @@
         <v>19</v>
       </c>
       <c r="B24" s="2">
-        <v>0.88</v>
+        <v>0.89</v>
       </c>
       <c r="C24" s="2">
-        <v>426195</v>
-      </c>
-      <c r="D24" s="6"/>
+        <v>145769</v>
+      </c>
+      <c r="D24" s="12"/>
       <c r="E24" s="1" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="F24" s="2">
-        <v>0.36</v>
+        <v>0.37</v>
       </c>
       <c r="G24" s="2">
-        <v>13885</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B25" s="8"/>
-      <c r="C25" s="9"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="F25" s="8"/>
-      <c r="G25" s="9"/>
-    </row>
-    <row r="26" spans="1:7" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B26" s="2">
-        <v>0.93</v>
-      </c>
-      <c r="C26" s="2">
-        <v>193916</v>
-      </c>
-      <c r="D26" s="6"/>
-      <c r="E26" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="F26" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="G26" s="2">
-        <v>27385</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B27" s="2">
-        <v>0.92</v>
-      </c>
-      <c r="C27" s="2">
-        <v>4610029</v>
-      </c>
-      <c r="D27" s="6"/>
-      <c r="E27" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F27" s="2">
-        <v>0.18</v>
-      </c>
-      <c r="G27" s="2">
-        <v>41158</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B28" s="2">
-        <v>0.92</v>
-      </c>
-      <c r="C28" s="2">
-        <v>84039</v>
-      </c>
-      <c r="D28" s="6"/>
-      <c r="E28" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="F28" s="2">
-        <v>0.21</v>
-      </c>
-      <c r="G28" s="2">
-        <v>13885</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B29" s="2">
-        <v>0.91</v>
-      </c>
-      <c r="C29" s="2">
-        <v>57420</v>
-      </c>
-      <c r="D29" s="6"/>
-      <c r="E29" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F29" s="2">
-        <v>0.22</v>
-      </c>
-      <c r="G29" s="2">
-        <v>30629</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B30" s="2">
-        <v>0.9</v>
-      </c>
-      <c r="C30" s="2">
-        <v>1979964</v>
-      </c>
-      <c r="D30" s="6"/>
-      <c r="E30" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F30" s="2">
-        <v>0.23</v>
-      </c>
-      <c r="G30" s="2">
-        <v>18628</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B31" s="2">
-        <v>0.9</v>
-      </c>
-      <c r="C31" s="2">
-        <v>1288629</v>
-      </c>
-      <c r="D31" s="6"/>
-      <c r="E31" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F31" s="2">
-        <v>0.26</v>
-      </c>
-      <c r="G31" s="2">
-        <v>43257</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B32" s="2">
-        <v>0.9</v>
-      </c>
-      <c r="C32" s="2">
-        <v>703548</v>
-      </c>
-      <c r="D32" s="6"/>
-      <c r="E32" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F32" s="2">
-        <v>0.31</v>
-      </c>
-      <c r="G32" s="2">
-        <v>51462</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B33" s="2">
-        <v>0.9</v>
-      </c>
-      <c r="C33" s="2">
-        <v>1565285</v>
-      </c>
-      <c r="D33" s="6"/>
-      <c r="E33" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F33" s="2">
-        <v>0.37</v>
-      </c>
-      <c r="G33" s="2">
-        <v>71464</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B34" s="2">
-        <v>0.89</v>
-      </c>
-      <c r="C34" s="2">
-        <v>19328</v>
-      </c>
-      <c r="D34" s="6"/>
-      <c r="E34" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F34" s="2">
-        <v>0.37</v>
-      </c>
-      <c r="G34" s="2">
         <v>29084</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B35" s="2">
-        <v>0.89</v>
-      </c>
-      <c r="C35" s="2">
-        <v>145769</v>
-      </c>
-      <c r="D35" s="6"/>
-      <c r="E35" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F35" s="2">
-        <v>0.38</v>
-      </c>
-      <c r="G35" s="2">
-        <v>177350</v>
-      </c>
-    </row>
+    <row r="25" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="6">
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="E1:G1"/>
     <mergeCell ref="A3:C3"/>
     <mergeCell ref="A14:C14"/>
-    <mergeCell ref="A25:C25"/>
     <mergeCell ref="E3:G3"/>
     <mergeCell ref="E14:G14"/>
-    <mergeCell ref="E25:G25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>